<commit_message>
6.1.1 ~ 6.1.5 추가함.
</commit_message>
<xml_diff>
--- a/1. [SE] SRS (& System testing).xlsx
+++ b/1. [SE] SRS (& System testing).xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werty\OneDrive\바탕 화면\SWP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83a6059c6a32dd14/바탕 화면/SWP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63641E96-244B-4C64-ADD8-6916D2DC5C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63641E96-244B-4C64-ADD8-6916D2DC5C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EA2F0FC-72D9-4FB5-A4FA-B636A41F0D28}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>1.1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -207,10 +207,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.1.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6.1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -224,6 +220,42 @@
   </si>
   <si>
     <t>6.1.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박창영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어플 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림, 진동 온오프 등 어플에서 제공하는 기능에 대한 설정을 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정 버튼을 눌러 어플 설정을 할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자가 설정을 바꾸면 바로 반영된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정에서 알림, 진동 on/off를 할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정에서 테마를 변경할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.1.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정에서 버전 정보를 알 수 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -949,6 +981,42 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1017,42 +1085,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1478,8 +1510,8 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1499,19 +1531,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="54"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="2"/>
@@ -1528,11 +1560,11 @@
       <c r="A3" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -1543,11 +1575,11 @@
       <c r="A4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -1573,8 +1605,12 @@
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="23">
+        <v>22311968</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -1645,74 +1681,74 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:11" s="24" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:11" s="25" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="76" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="55" t="s">
+      <c r="J14" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="55" t="s">
+      <c r="K14" s="67" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="25" customFormat="1" ht="16">
-      <c r="A15" s="59"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
     </row>
     <row r="16" spans="1:11" s="25" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
       <c r="H16" s="41"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="1:11" ht="16">
       <c r="A17" s="6">
@@ -2059,26 +2095,26 @@
       <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:11" ht="16">
-      <c r="A40" s="81">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B40" s="82"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="85"/>
+      <c r="A40" s="58">
+        <v>5</v>
+      </c>
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="62"/>
       <c r="G40" s="39"/>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" ht="16">
-      <c r="A41" s="30" t="s">
-        <v>39</v>
+      <c r="A41" s="30">
+        <v>5.0999999999999996</v>
       </c>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
-      <c r="D41" s="86"/>
+      <c r="D41" s="63"/>
       <c r="E41" s="49"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -2088,11 +2124,11 @@
     </row>
     <row r="42" spans="1:11" ht="16">
       <c r="A42" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
-      <c r="D42" s="86"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="49"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -2102,11 +2138,11 @@
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1">
       <c r="A43" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
-      <c r="D43" s="86"/>
+      <c r="D43" s="63"/>
       <c r="E43" s="49"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
@@ -2116,11 +2152,13 @@
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1">
       <c r="A44" s="30">
-        <v>6.1</v>
-      </c>
-      <c r="B44" s="30"/>
+        <v>6</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>46</v>
+      </c>
       <c r="C44" s="30"/>
-      <c r="D44" s="86"/>
+      <c r="D44" s="63"/>
       <c r="E44" s="49"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -2128,13 +2166,15 @@
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
     </row>
-    <row r="45" spans="1:11" ht="15" customHeight="1">
-      <c r="A45" s="30" t="s">
-        <v>42</v>
+    <row r="45" spans="1:11" ht="76.5" customHeight="1">
+      <c r="A45" s="30">
+        <v>6.1</v>
       </c>
       <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="86"/>
+      <c r="C45" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="63"/>
       <c r="E45" s="49"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -2144,11 +2184,12 @@
     </row>
     <row r="46" spans="1:11" ht="15" customHeight="1">
       <c r="A46" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="86"/>
+      <c r="D46" s="63" t="s">
+        <v>48</v>
+      </c>
       <c r="E46" s="49"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -2158,11 +2199,13 @@
     </row>
     <row r="47" spans="1:11" ht="15" customHeight="1">
       <c r="A47" s="30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
-      <c r="D47" s="86"/>
+      <c r="D47" s="63" t="s">
+        <v>49</v>
+      </c>
       <c r="E47" s="49"/>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -2172,11 +2215,13 @@
     </row>
     <row r="48" spans="1:11" ht="15" customHeight="1">
       <c r="A48" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
-      <c r="D48" s="86"/>
+      <c r="D48" s="63" t="s">
+        <v>50</v>
+      </c>
       <c r="E48" s="49"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
@@ -2185,10 +2230,14 @@
       <c r="K48" s="19"/>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1">
-      <c r="A49" s="30"/>
+      <c r="A49" s="30" t="s">
+        <v>44</v>
+      </c>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
-      <c r="D49" s="86"/>
+      <c r="D49" s="63" t="s">
+        <v>51</v>
+      </c>
       <c r="E49" s="49"/>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
@@ -2197,10 +2246,14 @@
       <c r="K49" s="19"/>
     </row>
     <row r="50" spans="1:11" ht="15" customHeight="1">
-      <c r="A50" s="30"/>
+      <c r="A50" s="30" t="s">
+        <v>52</v>
+      </c>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
-      <c r="D50" s="86"/>
+      <c r="D50" s="63" t="s">
+        <v>53</v>
+      </c>
       <c r="E50" s="49"/>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
@@ -2209,10 +2262,12 @@
       <c r="K50" s="19"/>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1">
-      <c r="A51" s="30"/>
+      <c r="A51" s="30">
+        <v>7</v>
+      </c>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
-      <c r="D51" s="86"/>
+      <c r="D51" s="63"/>
       <c r="E51" s="49"/>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
@@ -2224,7 +2279,7 @@
       <c r="A52" s="30"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
-      <c r="D52" s="86"/>
+      <c r="D52" s="63"/>
       <c r="E52" s="49"/>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
@@ -2236,7 +2291,7 @@
       <c r="A53" s="30"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
-      <c r="D53" s="86"/>
+      <c r="D53" s="63"/>
       <c r="E53" s="49"/>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
@@ -2248,7 +2303,7 @@
       <c r="A54" s="30"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
-      <c r="D54" s="86"/>
+      <c r="D54" s="63"/>
       <c r="E54" s="49"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
@@ -2260,7 +2315,7 @@
       <c r="A55" s="30"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
-      <c r="D55" s="86"/>
+      <c r="D55" s="63"/>
       <c r="E55" s="49"/>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
@@ -2272,7 +2327,7 @@
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
-      <c r="D56" s="86"/>
+      <c r="D56" s="63"/>
       <c r="E56" s="49"/>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
@@ -2284,7 +2339,7 @@
       <c r="A57" s="30"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
-      <c r="D57" s="86"/>
+      <c r="D57" s="63"/>
       <c r="E57" s="49"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
@@ -2296,7 +2351,7 @@
       <c r="A58" s="30"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
-      <c r="D58" s="86"/>
+      <c r="D58" s="63"/>
       <c r="E58" s="49"/>
       <c r="F58" s="19"/>
       <c r="G58" s="19"/>
@@ -2308,7 +2363,7 @@
       <c r="A59" s="30"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
-      <c r="D59" s="86"/>
+      <c r="D59" s="63"/>
       <c r="E59" s="49"/>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
@@ -2317,13 +2372,13 @@
       <c r="K59" s="19"/>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1" thickBot="1">
-      <c r="A60" s="75"/>
-      <c r="B60" s="76"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="78"/>
-      <c r="F60" s="79"/>
-      <c r="G60" s="80"/>
+      <c r="A60" s="52"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="57"/>
       <c r="I60" s="19"/>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>

</xml_diff>

<commit_message>
[SE] SRS (&System testing).xlsx 파일 수정함. 2,3,4,6번 기능 추가함
</commit_message>
<xml_diff>
--- a/1. [SE] SRS (& System testing).xlsx
+++ b/1. [SE] SRS (& System testing).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83a6059c6a32dd14/바탕 화면/SWP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63641E96-244B-4C64-ADD8-6916D2DC5C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EA2F0FC-72D9-4FB5-A4FA-B636A41F0D28}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{63641E96-244B-4C64-ADD8-6916D2DC5C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F239FF4-213F-4B59-805F-77CFB61695AA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Reference" sheetId="19" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">SRS!$A$1:$I$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">SRS!$A$1:$I$41</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">SRS!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>1.1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,66 +49,6 @@
   </si>
   <si>
     <t>eBL부가서비스 관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eBL Envelope 전자문서 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eBL Advice 전자문서 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eBL 전자문서 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.1.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eBL 전자문서 송신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eBL 전자문서 수신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.2.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BLEnvelope 전자문서 송신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShippingRequest 전자문서 수신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.1.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -199,14 +139,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5.1.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6.1.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -227,14 +159,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>어플 설정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알림, 진동 온오프 등 어플에서 제공하는 기능에 대한 설정을 한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>설정 버튼을 눌러 어플 설정을 할 수 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,6 +181,369 @@
   <si>
     <t>설정에서 버전 정보를 알 수 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>앱 연동하기</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>사용자는 이 앱을 이용해서 제한을 둘 앱을 연동한다.ex)유튜브, 인스타그램</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>앱 화면의 앱 연동하기를 클릭해서 연동시킬 앱을 정할 수 있다.</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>다수의 앱을 한번에 연동할 수 있다.</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>사용자가 직접 앱을 추가하거나 삭제 할 수 있다.</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>연동을 취소 하고 싶을 경우 사용자가 직접 취소 할 수 있다.</t>
+  </si>
+  <si>
+    <t>2.1.5</t>
+  </si>
+  <si>
+    <t>연동에 성공 할 경우 연동 중인 앱이 표시되게 한다.</t>
+  </si>
+  <si>
+    <t>2.1.6</t>
+  </si>
+  <si>
+    <t>연동된 앱의 알림 권한을 통합 관리한다.</t>
+  </si>
+  <si>
+    <t>2.1.7</t>
+  </si>
+  <si>
+    <t>어떤 앱이 언제 연동/해제 됬는지 기록 및 로그를 제공한다.</t>
+  </si>
+  <si>
+    <t>제한 기능</t>
+  </si>
+  <si>
+    <t>설정한 시간 이상 숏폼을 시청할 시 설정한 단계에 맞게 제한을 주는 기능이다.</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>제한 버튼을 눌러 제한하는 단계(수위)를 조절 할 수 있다.</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>사용자가 설정한 제한 단계가 즉시 반영된다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">제한 종류(시간, 영상 개수 중)를 원하는 단위로 설정할 수 있으며, 제한단계도 원하는 만큼 입력하여 설정할 수 있다.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">제한 강도(일정 시간마다 동기부여 글 띄워주기, 앱 종료 등)을 정할 수 있다. </t>
+  </si>
+  <si>
+    <t>최현준</t>
+  </si>
+  <si>
+    <t>김진수</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>커뮤니티 기능</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>커뮤니티 글 작성</t>
+  </si>
+  <si>
+    <t>사용자는 커뮤니티에 글을 작성할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>사용자가 커뮤니티에 접속하여 "글 작성" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>사용자가 글을 작성하고 "작성 완료" 버튼을 누르면 커뮤니티에 글이 게시된다.</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>사용자가 글 내용을 작성하지 않으면 빈 내용은 등록할 수 없다는 에러 메시지를 띄운다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 글 삭제</t>
+  </si>
+  <si>
+    <t>사용자는 커뮤니티에 작성한 자신의 글을 삭제할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>사용자가 커뮤니티에 작성한 자신의 글을 클릭하여 "글 삭제" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>사용자가 "글 삭제" 버튼을 누르면 커뮤니티에서 사용자가 게시한 글이 사라진다.</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>사용자는 본인의 글이 아닌 글을 클릭했을 경우에는 "글 삭제" 버튼이 비활성화된다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 댓글 작성</t>
+  </si>
+  <si>
+    <t>사용자는 커뮤니티 글에 댓글을 작성하여 등록할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>사용자가 댓글을 작성하고자 하는 글을 클릭한다.</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>사용자가 댓글창에 댓글을 작성한 후 "댓글 작성" 버튼을 누르면 댓글이 게시된다.</t>
+  </si>
+  <si>
+    <t>3.3.3</t>
+  </si>
+  <si>
+    <t>사용자가 댓글 내용을 작성하지 않으면 빈 내용은 등록할 수 없다는 에러 메시지를 띄운다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 댓글 삭제</t>
+  </si>
+  <si>
+    <t>사용자는 커뮤니티 글에 작성한 댓글을 삭제할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>사용자가 커뮤니티에 작성한 자신의 댓글 옆에 있는 "댓글 삭제" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.4.2</t>
+  </si>
+  <si>
+    <t>사용자가 "댓글 삭제" 버튼을 누르면 커뮤니티에서 사용자가 게시한 댓글이 사라진다.</t>
+  </si>
+  <si>
+    <t>3.4.3</t>
+  </si>
+  <si>
+    <t>사용자가 작성한 댓글이 아닌 경우에는 "댓글 삭제" 버튼이 비활성화 되어 삭제할 수 없다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 글 추천 기능</t>
+  </si>
+  <si>
+    <t>사용자는 자신의 마음에 든 글에 추천을 할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.5.1</t>
+  </si>
+  <si>
+    <t>사용자가 마음에 든 글이 있으면 "추천" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.5.2</t>
+  </si>
+  <si>
+    <t>사용자의 추천 버튼을 누른 글의 추천 표시 옆에 있는 추천 수가 올라간다.</t>
+  </si>
+  <si>
+    <t>3.5.3</t>
+  </si>
+  <si>
+    <t>사용자가 이미 추천 버튼을 누른 글은 또다시 추천 버튼을 누를 수 없다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 댓글 추천 기능</t>
+  </si>
+  <si>
+    <t>사용자는 자신의 마음에 든 댓글에 추천을 할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.6.1</t>
+  </si>
+  <si>
+    <t>사용자가 마음에 든 댓글이 있으면 "추천" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.6.2</t>
+  </si>
+  <si>
+    <t>사용자의 추천 버튼을 누른 댓글의 추천 표시 옆에 있는 추천 수가 올라간다.</t>
+  </si>
+  <si>
+    <t>3.6.3</t>
+  </si>
+  <si>
+    <t>사용자가 이미 추천 버튼을 누른 댓글은 또다시 추천 버튼을 누를 수 없다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 글 신고</t>
+  </si>
+  <si>
+    <t>사용자는 커뮤니티에 게시된 부적절한 글을 신고할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.7.1</t>
+  </si>
+  <si>
+    <t>사용자가 부적절하다고 생각되는 글에 있는 "신고" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.7.2</t>
+  </si>
+  <si>
+    <t>사용자가 신고 버튼을 누른 글이 관리자에게 접수된다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 댓글 신고</t>
+  </si>
+  <si>
+    <t>사용자는 커뮤니티에 게시된 부적절한 댓글을 신고할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.8.1</t>
+  </si>
+  <si>
+    <t>사용자가 부적절하다고 생각되는 댓글에 있는 "신고" 버튼을 누른다.</t>
+  </si>
+  <si>
+    <t>3.8.2</t>
+  </si>
+  <si>
+    <t>사용자가 신고 버튼을 누른 댓글이 관리자에게 접수된다.</t>
+  </si>
+  <si>
+    <t>커뮤니티 신고 글/댓글 관리</t>
+  </si>
+  <si>
+    <t>관리자는 사용자들이 신고한 글/댓글의 내용을 보고 삭제할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.9.1</t>
+  </si>
+  <si>
+    <t>관리자는 사용자가 신고한 글/댓글 목록을 확인할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.9.2</t>
+  </si>
+  <si>
+    <t>관리자는 신고된 글/댓글에서 유해하거나 부적절한 내용이 있다면 관리자 권한으로 해당 글/댓글을 삭제할 수 있다.</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>연동 한 앱의 쇼츠 릴스 영상을 자동으로 감지한다.</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>남은 시간/영상 갯수를 앱 내 실시간으로 보여준다.</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>특정 시간대만 제한 할 수 있는 옵션을 제공한다.</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
+  <si>
+    <t>임의 해제 방지를 위해 기능을 추가한다.</t>
+  </si>
+  <si>
+    <t>2.2.5</t>
+  </si>
+  <si>
+    <t>앱 연동 후 제한 조건 설정하기를 눌러 영상 갯수, 시간 중에 한가지를 선택한다.</t>
+  </si>
+  <si>
+    <t>2.2.6</t>
+  </si>
+  <si>
+    <t>앱별로 최대 시청 시간을 설정한다. 단위는 5분 단위이다.(쇼츠 또는 릴스)</t>
+  </si>
+  <si>
+    <t>2.2.7</t>
+  </si>
+  <si>
+    <t>앱별로 시청 가능 영상 갯수를 설정한다. 단위는 3개이다. (쇼츠 또는 릴스)</t>
+  </si>
+  <si>
+    <t>제한 조건 설정(영상 갯수,시간)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">사용자가 본인이 원하는 방식으로 제한 조건을 설정한다. </t>
+  </si>
+  <si>
+    <t>조수현</t>
+  </si>
+  <si>
+    <t>어플 설정</t>
+  </si>
+  <si>
+    <t>알림, 진동 온오프 등 어플에서 제공하는 기능에 대한 설정을 한다.</t>
   </si>
 </sst>
 </file>
@@ -266,7 +553,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -350,6 +637,13 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -383,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -818,13 +1112,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -903,9 +1274,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -916,9 +1284,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -981,33 +1346,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1086,10 +1424,113 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal_Extraordinary Expense" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="3" xr:uid="{6D86845A-E37A-4290-AFE8-3B0F1C32CD47}"/>
     <cellStyle name="표준_온라인테스트-문제점-단체의료" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1508,10 +1949,10 @@
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1531,19 +1972,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
+      <c r="A1" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="55"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="2"/>
@@ -1558,13 +1999,13 @@
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="85" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+        <v>21</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -1573,13 +2014,13 @@
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="115.5" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
+        <v>5</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -1588,13 +2029,13 @@
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -1609,7 +2050,7 @@
         <v>22311968</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -1620,8 +2061,12 @@
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="23">
+        <v>22112124</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -1631,8 +2076,12 @@
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="23">
+        <v>22012061</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>62</v>
+      </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1641,7 +2090,12 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:11" s="23" customFormat="1" ht="15" customHeight="1">
-      <c r="C9" s="22"/>
+      <c r="B9" s="93">
+        <v>22112050</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>153</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1681,74 +2135,74 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:11" s="24" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A13" s="86" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
+      <c r="A13" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:11" s="25" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A14" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="76" t="s">
-        <v>23</v>
+      <c r="A14" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="65" t="s">
+        <v>8</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="67" t="s">
-        <v>25</v>
+      <c r="I14" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="56" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="25" customFormat="1" ht="16">
-      <c r="A15" s="71"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
     </row>
     <row r="16" spans="1:11" s="25" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A16" s="72"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
     </row>
     <row r="17" spans="1:11" ht="16">
       <c r="A17" s="6">
@@ -1759,8 +2213,8 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="34"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="8"/>
       <c r="H17" s="12"/>
       <c r="I17" s="8"/>
@@ -1776,8 +2230,8 @@
         <v>3</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="35"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
       <c r="I18" s="11"/>
@@ -1791,9 +2245,9 @@
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="21"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="42"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="12"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -1804,9 +2258,9 @@
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="42"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="12"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -1819,8 +2273,8 @@
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="11"/>
       <c r="H21" s="12"/>
       <c r="I21" s="19"/>
@@ -1828,27 +2282,27 @@
       <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" ht="36" customHeight="1" outlineLevel="1">
-      <c r="A22" s="28"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="29"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="43"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:11" s="40" customFormat="1" ht="84" customHeight="1" outlineLevel="1">
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+    </row>
+    <row r="23" spans="1:11" s="38" customFormat="1" ht="84" customHeight="1" outlineLevel="1">
       <c r="A23" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="10"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="11"/>
       <c r="H23" s="21"/>
       <c r="I23" s="19"/>
@@ -1856,105 +2310,115 @@
       <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" ht="16">
-      <c r="A24" s="32">
-        <v>2</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="38"/>
+      <c r="A24" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="27"/>
+      <c r="H24" s="26"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" spans="1:11" ht="32">
-      <c r="A25" s="32">
-        <v>2.1</v>
-      </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="38"/>
+    <row r="25" spans="1:11" ht="64">
+      <c r="A25" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="36"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="27"/>
+      <c r="H25" s="26"/>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A26" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="50"/>
+      <c r="A26" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="48"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="27"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="19"/>
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="144" customHeight="1" outlineLevel="1">
-      <c r="A27" s="32"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="38"/>
+      <c r="A27" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="49"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="27"/>
+      <c r="H27" s="26"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="45.75" customHeight="1" outlineLevel="1">
-      <c r="A28" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="38"/>
+      <c r="A28" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="48"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
     <row r="29" spans="1:11" ht="32">
-      <c r="A29" s="32">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="38"/>
+      <c r="A29" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="47"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="1:11" ht="45.75" customHeight="1" outlineLevel="1">
-      <c r="A30" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="50"/>
+      <c r="A30" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="48"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="I30" s="19"/>
@@ -1962,426 +2426,1280 @@
       <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" ht="38.25" customHeight="1" outlineLevel="1">
-      <c r="A31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="38"/>
+      <c r="A31" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="48"/>
+      <c r="F31" s="36"/>
       <c r="G31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" ht="16">
-      <c r="A32" s="32">
-        <v>3</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="38"/>
+    <row r="32" spans="1:11" ht="32">
+      <c r="A32" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="47"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="19"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" ht="32">
-      <c r="A33" s="32">
-        <v>3.1</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="49"/>
-      <c r="F33" s="38"/>
+    <row r="33" spans="1:11" ht="48">
+      <c r="A33" s="95">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B33" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="105"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:11" ht="34.5" customHeight="1" outlineLevel="1">
-      <c r="A34" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="38"/>
+      <c r="A34" s="95" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="105" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="100"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" ht="40.5" customHeight="1" outlineLevel="1">
-      <c r="A35" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="38"/>
+      <c r="A35" s="95" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="105" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="100"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
     </row>
-    <row r="36" spans="1:11" ht="16">
-      <c r="A36" s="31">
-        <v>4</v>
-      </c>
-      <c r="B36" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="38"/>
+    <row r="36" spans="1:11" ht="32">
+      <c r="A36" s="95" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="82"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="K36" s="19"/>
     </row>
-    <row r="37" spans="1:11" ht="32">
-      <c r="A37" s="31">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="38"/>
+    <row r="37" spans="1:11" ht="16">
+      <c r="A37" s="95" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="105" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="82"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="19"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" ht="48" customHeight="1" outlineLevel="1">
-      <c r="A38" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="38"/>
+      <c r="A38" s="95" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="95"/>
+      <c r="C38" s="95"/>
+      <c r="D38" s="105" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="100"/>
+      <c r="F38" s="36"/>
       <c r="G38" s="19"/>
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="19"/>
     </row>
     <row r="39" spans="1:11" ht="40.5" customHeight="1" outlineLevel="1">
-      <c r="A39" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="38"/>
+      <c r="A39" s="95" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="95"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="105" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="100"/>
+      <c r="F39" s="36"/>
       <c r="G39" s="19"/>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
     </row>
-    <row r="40" spans="1:11" ht="16">
-      <c r="A40" s="58">
-        <v>5</v>
-      </c>
-      <c r="B40" s="59"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="39"/>
+    <row r="40" spans="1:11" ht="32">
+      <c r="A40" s="95" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="95"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="105" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="85"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="37"/>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" ht="16">
-      <c r="A41" s="30">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="49"/>
+      <c r="A41" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="84"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="47"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
     </row>
-    <row r="42" spans="1:11" ht="16">
-      <c r="A42" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="49"/>
+    <row r="42" spans="1:11" ht="32">
+      <c r="A42" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="91"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
     </row>
-    <row r="43" spans="1:11" ht="15" customHeight="1">
-      <c r="A43" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="49"/>
+    <row r="43" spans="1:11" ht="43" customHeight="1">
+      <c r="A43" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="88"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="82"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
       <c r="I43" s="19"/>
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
     </row>
-    <row r="44" spans="1:11" ht="15" customHeight="1">
-      <c r="A44" s="30">
-        <v>6</v>
-      </c>
-      <c r="B44" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="49"/>
+    <row r="44" spans="1:11" ht="44.5" customHeight="1">
+      <c r="A44" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="82"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
     </row>
-    <row r="45" spans="1:11" ht="76.5" customHeight="1">
-      <c r="A45" s="30">
-        <v>6.1</v>
-      </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="63"/>
-      <c r="E45" s="49"/>
+    <row r="45" spans="1:11" ht="48" customHeight="1">
+      <c r="A45" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="88"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="82"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
       <c r="I45" s="19"/>
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
     </row>
-    <row r="46" spans="1:11" ht="15" customHeight="1">
-      <c r="A46" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="30"/>
-      <c r="D46" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" s="49"/>
+    <row r="46" spans="1:11" ht="53.5" customHeight="1">
+      <c r="A46" s="87" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="98" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="104"/>
+      <c r="E46" s="82"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
       <c r="I46" s="19"/>
       <c r="J46" s="19"/>
       <c r="K46" s="19"/>
     </row>
-    <row r="47" spans="1:11" ht="15" customHeight="1">
-      <c r="A47" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="49"/>
+    <row r="47" spans="1:11" ht="38" customHeight="1">
+      <c r="A47" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="95"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="82"/>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
       <c r="K47" s="19"/>
     </row>
-    <row r="48" spans="1:11" ht="15" customHeight="1">
-      <c r="A48" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="49"/>
+    <row r="48" spans="1:11" ht="33" customHeight="1">
+      <c r="A48" s="97" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="95"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="82"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
       <c r="I48" s="19"/>
       <c r="J48" s="19"/>
       <c r="K48" s="19"/>
     </row>
-    <row r="49" spans="1:11" ht="15" customHeight="1">
-      <c r="A49" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="49"/>
+    <row r="49" spans="1:11" ht="32" customHeight="1">
+      <c r="A49" s="97" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="82"/>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
       <c r="I49" s="19"/>
       <c r="J49" s="19"/>
       <c r="K49" s="19"/>
     </row>
-    <row r="50" spans="1:11" ht="15" customHeight="1">
-      <c r="A50" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="E50" s="49"/>
+    <row r="50" spans="1:11" ht="69.5" customHeight="1">
+      <c r="A50" s="87" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="88" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="104"/>
+      <c r="E50" s="82"/>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
       <c r="I50" s="19"/>
       <c r="J50" s="19"/>
       <c r="K50" s="19"/>
     </row>
-    <row r="51" spans="1:11" ht="15" customHeight="1">
-      <c r="A51" s="30">
-        <v>7</v>
-      </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="49"/>
+    <row r="51" spans="1:11" ht="33" customHeight="1">
+      <c r="A51" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="88"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51" s="47"/>
       <c r="F51" s="19"/>
       <c r="G51" s="19"/>
       <c r="I51" s="19"/>
       <c r="J51" s="19"/>
       <c r="K51" s="19"/>
     </row>
-    <row r="52" spans="1:11" ht="15" customHeight="1">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="49"/>
+    <row r="52" spans="1:11" ht="45.5" customHeight="1">
+      <c r="A52" s="87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="88"/>
+      <c r="C52" s="88"/>
+      <c r="D52" s="91" t="s">
+        <v>87</v>
+      </c>
+      <c r="E52" s="47"/>
       <c r="F52" s="19"/>
       <c r="G52" s="19"/>
       <c r="I52" s="19"/>
       <c r="J52" s="19"/>
       <c r="K52" s="19"/>
     </row>
-    <row r="53" spans="1:11" ht="15" customHeight="1">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="49"/>
+    <row r="53" spans="1:11" ht="70" customHeight="1">
+      <c r="A53" s="87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="88"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="47"/>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
       <c r="I53" s="19"/>
       <c r="J53" s="19"/>
       <c r="K53" s="19"/>
     </row>
-    <row r="54" spans="1:11" ht="15" customHeight="1">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="63"/>
-      <c r="E54" s="49"/>
+    <row r="54" spans="1:11" ht="54.5" customHeight="1">
+      <c r="A54" s="87" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="104"/>
+      <c r="E54" s="47"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
       <c r="I54" s="19"/>
       <c r="J54" s="19"/>
       <c r="K54" s="19"/>
     </row>
-    <row r="55" spans="1:11" ht="15" customHeight="1">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="49"/>
+    <row r="55" spans="1:11" ht="34.5" customHeight="1">
+      <c r="A55" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="95"/>
+      <c r="C55" s="95"/>
+      <c r="D55" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="47"/>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
       <c r="I55" s="19"/>
       <c r="J55" s="19"/>
       <c r="K55" s="19"/>
     </row>
-    <row r="56" spans="1:11" ht="15" customHeight="1">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="49"/>
+    <row r="56" spans="1:11" ht="32" customHeight="1">
+      <c r="A56" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="95"/>
+      <c r="C56" s="95"/>
+      <c r="D56" s="98" t="s">
+        <v>95</v>
+      </c>
+      <c r="E56" s="47"/>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
       <c r="I56" s="19"/>
       <c r="J56" s="19"/>
       <c r="K56" s="19"/>
     </row>
-    <row r="57" spans="1:11" ht="15" customHeight="1">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="49"/>
+    <row r="57" spans="1:11" ht="47" customHeight="1">
+      <c r="A57" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="95"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="47"/>
       <c r="F57" s="19"/>
       <c r="G57" s="19"/>
       <c r="I57" s="19"/>
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
     </row>
-    <row r="58" spans="1:11" ht="15" customHeight="1">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="49"/>
+    <row r="58" spans="1:11" ht="55" customHeight="1">
+      <c r="A58" s="97" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="98"/>
+      <c r="E58" s="47"/>
       <c r="F58" s="19"/>
       <c r="G58" s="19"/>
       <c r="I58" s="19"/>
       <c r="J58" s="19"/>
       <c r="K58" s="19"/>
     </row>
-    <row r="59" spans="1:11" ht="15" customHeight="1">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
+    <row r="59" spans="1:11" ht="48" customHeight="1">
+      <c r="A59" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="95"/>
+      <c r="C59" s="95"/>
+      <c r="D59" s="98" t="s">
+        <v>101</v>
+      </c>
+      <c r="E59" s="76"/>
+      <c r="F59" s="77"/>
+      <c r="G59" s="78"/>
       <c r="I59" s="19"/>
       <c r="J59" s="19"/>
       <c r="K59" s="19"/>
     </row>
-    <row r="60" spans="1:11" ht="15" customHeight="1" thickBot="1">
-      <c r="A60" s="52"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="54"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="57"/>
+    <row r="60" spans="1:11" ht="36.5" customHeight="1">
+      <c r="A60" s="96" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="95"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="50"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="37"/>
       <c r="I60" s="19"/>
       <c r="J60" s="19"/>
       <c r="K60" s="19"/>
+    </row>
+    <row r="61" spans="1:11" ht="36.5" customHeight="1">
+      <c r="A61" s="96" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
+      <c r="D61" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" s="50"/>
+      <c r="F61" s="81"/>
+      <c r="G61" s="81"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+    </row>
+    <row r="62" spans="1:11" ht="49" customHeight="1">
+      <c r="A62" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="D62" s="98"/>
+      <c r="E62" s="80"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="37"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+    </row>
+    <row r="63" spans="1:11" ht="37" customHeight="1">
+      <c r="A63" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="95"/>
+      <c r="C63" s="95"/>
+      <c r="D63" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" s="80"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+    </row>
+    <row r="64" spans="1:11" ht="31.5" customHeight="1">
+      <c r="A64" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" s="95"/>
+      <c r="C64" s="95"/>
+      <c r="D64" s="94" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" s="80"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+    </row>
+    <row r="65" spans="1:11" ht="33" customHeight="1">
+      <c r="A65" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="95"/>
+      <c r="C65" s="95"/>
+      <c r="D65" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="E65" s="80"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" spans="1:11" ht="48" customHeight="1">
+      <c r="A66" s="101">
+        <v>3.7</v>
+      </c>
+      <c r="B66" s="102" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="102" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" s="103"/>
+      <c r="E66" s="80"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+    </row>
+    <row r="67" spans="1:11" ht="38.5" customHeight="1">
+      <c r="A67" s="101" t="s">
+        <v>116</v>
+      </c>
+      <c r="B67" s="102"/>
+      <c r="C67" s="102"/>
+      <c r="D67" s="103" t="s">
+        <v>117</v>
+      </c>
+      <c r="E67" s="80"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+    </row>
+    <row r="68" spans="1:11" ht="38.5" customHeight="1">
+      <c r="A68" s="101" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="102"/>
+      <c r="C68" s="102"/>
+      <c r="D68" s="103" t="s">
+        <v>119</v>
+      </c>
+      <c r="E68" s="80"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
+      <c r="K68" s="19"/>
+    </row>
+    <row r="69" spans="1:11" ht="50.5" customHeight="1">
+      <c r="A69" s="101">
+        <v>3.8</v>
+      </c>
+      <c r="B69" s="102" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="102" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" s="103"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="19"/>
+      <c r="K69" s="19"/>
+    </row>
+    <row r="70" spans="1:11" ht="32.5" customHeight="1">
+      <c r="A70" s="101" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" s="102"/>
+      <c r="C70" s="102"/>
+      <c r="D70" s="103" t="s">
+        <v>123</v>
+      </c>
+      <c r="E70" s="80"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="19"/>
+      <c r="K70" s="19"/>
+    </row>
+    <row r="71" spans="1:11" ht="39.5" customHeight="1">
+      <c r="A71" s="101" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="102"/>
+      <c r="C71" s="102"/>
+      <c r="D71" s="103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E71" s="80"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
+      <c r="K71" s="19"/>
+    </row>
+    <row r="72" spans="1:11" ht="68.5" customHeight="1">
+      <c r="A72" s="101">
+        <v>3.9</v>
+      </c>
+      <c r="B72" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="102" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" s="103"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="19"/>
+      <c r="K72" s="19"/>
+    </row>
+    <row r="73" spans="1:11" ht="31.5" customHeight="1">
+      <c r="A73" s="101" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" s="102"/>
+      <c r="C73" s="102"/>
+      <c r="D73" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="E73" s="80"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="19"/>
+    </row>
+    <row r="74" spans="1:11" ht="47.5" customHeight="1">
+      <c r="A74" s="101" t="s">
+        <v>130</v>
+      </c>
+      <c r="B74" s="102"/>
+      <c r="C74" s="102"/>
+      <c r="D74" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="E74" s="80"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="19"/>
+    </row>
+    <row r="75" spans="1:11" ht="15" customHeight="1">
+      <c r="A75" s="95">
+        <v>4</v>
+      </c>
+      <c r="B75" s="95" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" s="95"/>
+      <c r="D75" s="52"/>
+      <c r="E75" s="80"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+    </row>
+    <row r="76" spans="1:11" ht="63" customHeight="1">
+      <c r="A76" s="95">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B76" s="95"/>
+      <c r="C76" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="D76" s="52"/>
+      <c r="E76" s="80"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+    </row>
+    <row r="77" spans="1:11" ht="42.5" customHeight="1">
+      <c r="A77" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77" s="95"/>
+      <c r="C77" s="95"/>
+      <c r="D77" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="E77" s="80"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
+      <c r="K77" s="19"/>
+    </row>
+    <row r="78" spans="1:11" ht="39.5" customHeight="1">
+      <c r="A78" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78" s="95"/>
+      <c r="C78" s="95"/>
+      <c r="D78" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E78" s="80"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+      <c r="K78" s="19"/>
+    </row>
+    <row r="79" spans="1:11" ht="52.5" customHeight="1">
+      <c r="A79" s="95">
+        <v>4.13</v>
+      </c>
+      <c r="B79" s="95"/>
+      <c r="C79" s="95"/>
+      <c r="D79" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79" s="80"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
+    </row>
+    <row r="80" spans="1:11" ht="42" customHeight="1">
+      <c r="A80" s="95">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="B80" s="95"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="E80" s="80"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+    </row>
+    <row r="81" spans="1:11" ht="15" customHeight="1">
+      <c r="A81" s="95">
+        <v>5</v>
+      </c>
+      <c r="B81" s="79"/>
+      <c r="C81" s="79"/>
+      <c r="D81" s="83"/>
+      <c r="E81" s="99"/>
+      <c r="F81" s="81"/>
+      <c r="G81" s="81"/>
+      <c r="I81" s="90"/>
+      <c r="J81" s="90"/>
+      <c r="K81" s="90"/>
+    </row>
+    <row r="82" spans="1:11" ht="15" customHeight="1">
+      <c r="A82" s="79"/>
+      <c r="B82" s="79"/>
+      <c r="C82" s="79"/>
+      <c r="D82" s="83"/>
+      <c r="E82" s="99"/>
+      <c r="F82" s="81"/>
+      <c r="G82" s="107"/>
+      <c r="I82" s="90"/>
+      <c r="J82" s="90"/>
+      <c r="K82" s="90"/>
+    </row>
+    <row r="83" spans="1:11" ht="15" customHeight="1">
+      <c r="A83" s="79"/>
+      <c r="B83" s="79"/>
+      <c r="C83" s="79"/>
+      <c r="D83" s="83"/>
+      <c r="E83" s="99"/>
+      <c r="F83" s="81"/>
+      <c r="G83" s="108"/>
+      <c r="I83" s="90"/>
+      <c r="J83" s="90"/>
+      <c r="K83" s="90"/>
+    </row>
+    <row r="84" spans="1:11" ht="15" customHeight="1">
+      <c r="A84" s="79"/>
+      <c r="B84" s="79"/>
+      <c r="C84" s="79"/>
+      <c r="D84" s="83"/>
+      <c r="E84" s="99"/>
+      <c r="F84" s="81"/>
+      <c r="G84" s="108"/>
+      <c r="I84" s="90"/>
+      <c r="J84" s="90"/>
+      <c r="K84" s="90"/>
+    </row>
+    <row r="85" spans="1:11" ht="15" customHeight="1">
+      <c r="A85" s="79"/>
+      <c r="B85" s="79"/>
+      <c r="C85" s="79"/>
+      <c r="D85" s="83"/>
+      <c r="E85" s="99"/>
+      <c r="F85" s="81"/>
+      <c r="G85" s="108"/>
+      <c r="I85" s="90"/>
+      <c r="J85" s="90"/>
+      <c r="K85" s="90"/>
+    </row>
+    <row r="86" spans="1:11" ht="15" customHeight="1">
+      <c r="A86" s="79"/>
+      <c r="B86" s="79"/>
+      <c r="C86" s="79"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="99"/>
+      <c r="F86" s="81"/>
+      <c r="G86" s="108"/>
+      <c r="I86" s="90"/>
+      <c r="J86" s="90"/>
+      <c r="K86" s="90"/>
+    </row>
+    <row r="87" spans="1:11" ht="15" customHeight="1">
+      <c r="A87" s="79"/>
+      <c r="B87" s="79"/>
+      <c r="C87" s="79"/>
+      <c r="D87" s="83"/>
+      <c r="E87" s="99"/>
+      <c r="F87" s="81"/>
+      <c r="G87" s="108"/>
+      <c r="I87" s="90"/>
+      <c r="J87" s="90"/>
+      <c r="K87" s="90"/>
+    </row>
+    <row r="88" spans="1:11" ht="15" customHeight="1">
+      <c r="A88" s="79"/>
+      <c r="B88" s="79"/>
+      <c r="C88" s="79"/>
+      <c r="D88" s="83"/>
+      <c r="E88" s="99"/>
+      <c r="F88" s="81"/>
+      <c r="G88" s="108"/>
+      <c r="I88" s="90"/>
+      <c r="J88" s="90"/>
+      <c r="K88" s="90"/>
+    </row>
+    <row r="89" spans="1:11" ht="15" customHeight="1">
+      <c r="A89" s="79"/>
+      <c r="B89" s="79"/>
+      <c r="C89" s="79"/>
+      <c r="D89" s="83"/>
+      <c r="E89" s="99"/>
+      <c r="F89" s="81"/>
+      <c r="G89" s="108"/>
+      <c r="I89" s="90"/>
+      <c r="J89" s="90"/>
+      <c r="K89" s="90"/>
+    </row>
+    <row r="90" spans="1:11" ht="15" customHeight="1">
+      <c r="A90" s="79"/>
+      <c r="B90" s="79"/>
+      <c r="C90" s="79"/>
+      <c r="D90" s="83"/>
+      <c r="E90" s="99"/>
+      <c r="F90" s="81"/>
+      <c r="G90" s="108"/>
+      <c r="I90" s="90"/>
+      <c r="J90" s="90"/>
+      <c r="K90" s="90"/>
+    </row>
+    <row r="91" spans="1:11" ht="15" customHeight="1">
+      <c r="A91" s="79"/>
+      <c r="B91" s="79"/>
+      <c r="C91" s="79"/>
+      <c r="D91" s="83"/>
+      <c r="E91" s="99"/>
+      <c r="F91" s="81"/>
+      <c r="G91" s="108"/>
+      <c r="I91" s="90"/>
+      <c r="J91" s="90"/>
+      <c r="K91" s="90"/>
+    </row>
+    <row r="92" spans="1:11" ht="15" customHeight="1">
+      <c r="A92" s="79"/>
+      <c r="B92" s="79"/>
+      <c r="C92" s="79"/>
+      <c r="D92" s="83"/>
+      <c r="E92" s="99"/>
+      <c r="F92" s="81"/>
+      <c r="G92" s="108"/>
+      <c r="I92" s="90"/>
+      <c r="J92" s="90"/>
+      <c r="K92" s="90"/>
+    </row>
+    <row r="93" spans="1:11" ht="15" customHeight="1">
+      <c r="A93" s="79"/>
+      <c r="B93" s="79"/>
+      <c r="C93" s="79"/>
+      <c r="D93" s="83"/>
+      <c r="E93" s="99"/>
+      <c r="F93" s="81"/>
+      <c r="G93" s="108"/>
+      <c r="I93" s="90"/>
+      <c r="J93" s="90"/>
+      <c r="K93" s="90"/>
+    </row>
+    <row r="94" spans="1:11" ht="15" customHeight="1">
+      <c r="A94" s="79"/>
+      <c r="B94" s="79"/>
+      <c r="C94" s="79"/>
+      <c r="D94" s="83"/>
+      <c r="E94" s="99"/>
+      <c r="F94" s="81"/>
+      <c r="G94" s="108"/>
+      <c r="I94" s="90"/>
+      <c r="J94" s="90"/>
+      <c r="K94" s="90"/>
+    </row>
+    <row r="95" spans="1:11" ht="15" customHeight="1">
+      <c r="A95" s="79"/>
+      <c r="B95" s="79"/>
+      <c r="C95" s="79"/>
+      <c r="D95" s="83"/>
+      <c r="E95" s="99"/>
+      <c r="F95" s="81"/>
+      <c r="G95" s="108"/>
+      <c r="I95" s="90"/>
+      <c r="J95" s="90"/>
+      <c r="K95" s="90"/>
+    </row>
+    <row r="96" spans="1:11" ht="15" customHeight="1">
+      <c r="A96" s="79"/>
+      <c r="B96" s="79"/>
+      <c r="C96" s="79"/>
+      <c r="D96" s="83"/>
+      <c r="E96" s="99"/>
+      <c r="F96" s="81"/>
+      <c r="G96" s="108"/>
+      <c r="I96" s="90"/>
+      <c r="J96" s="90"/>
+      <c r="K96" s="90"/>
+    </row>
+    <row r="97" spans="1:11" ht="15" customHeight="1">
+      <c r="A97" s="79"/>
+      <c r="B97" s="79"/>
+      <c r="C97" s="79"/>
+      <c r="D97" s="83"/>
+      <c r="E97" s="99"/>
+      <c r="F97" s="81"/>
+      <c r="G97" s="108"/>
+      <c r="I97" s="90"/>
+      <c r="J97" s="90"/>
+      <c r="K97" s="90"/>
+    </row>
+    <row r="98" spans="1:11" ht="15" customHeight="1">
+      <c r="A98" s="79"/>
+      <c r="B98" s="79"/>
+      <c r="C98" s="79"/>
+      <c r="D98" s="83"/>
+      <c r="E98" s="99"/>
+      <c r="F98" s="81"/>
+      <c r="G98" s="108"/>
+      <c r="I98" s="90"/>
+      <c r="J98" s="90"/>
+      <c r="K98" s="90"/>
+    </row>
+    <row r="99" spans="1:11" ht="15" customHeight="1">
+      <c r="A99" s="79"/>
+      <c r="B99" s="79"/>
+      <c r="C99" s="79"/>
+      <c r="D99" s="83"/>
+      <c r="E99" s="99"/>
+      <c r="F99" s="81"/>
+      <c r="G99" s="108"/>
+      <c r="I99" s="90"/>
+      <c r="J99" s="90"/>
+      <c r="K99" s="90"/>
+    </row>
+    <row r="100" spans="1:11" ht="15" customHeight="1">
+      <c r="A100" s="79"/>
+      <c r="B100" s="79"/>
+      <c r="C100" s="79"/>
+      <c r="D100" s="83"/>
+      <c r="E100" s="99"/>
+      <c r="F100" s="81"/>
+      <c r="G100" s="108"/>
+      <c r="I100" s="90"/>
+      <c r="J100" s="90"/>
+      <c r="K100" s="90"/>
+    </row>
+    <row r="101" spans="1:11" ht="15" customHeight="1">
+      <c r="A101" s="79"/>
+      <c r="B101" s="79"/>
+      <c r="C101" s="79"/>
+      <c r="D101" s="83"/>
+      <c r="E101" s="99"/>
+      <c r="F101" s="81"/>
+      <c r="G101" s="108"/>
+      <c r="I101" s="90"/>
+      <c r="J101" s="90"/>
+      <c r="K101" s="90"/>
+    </row>
+    <row r="102" spans="1:11" ht="15" customHeight="1">
+      <c r="A102" s="79"/>
+      <c r="B102" s="79"/>
+      <c r="C102" s="79"/>
+      <c r="D102" s="83"/>
+      <c r="E102" s="99"/>
+      <c r="F102" s="81"/>
+      <c r="G102" s="108"/>
+      <c r="I102" s="90"/>
+      <c r="J102" s="90"/>
+      <c r="K102" s="90"/>
+    </row>
+    <row r="103" spans="1:11" ht="15" customHeight="1">
+      <c r="A103" s="79"/>
+      <c r="B103" s="79"/>
+      <c r="C103" s="79"/>
+      <c r="D103" s="83"/>
+      <c r="E103" s="99"/>
+      <c r="F103" s="81"/>
+      <c r="G103" s="108"/>
+      <c r="I103" s="90"/>
+      <c r="J103" s="90"/>
+      <c r="K103" s="90"/>
+    </row>
+    <row r="104" spans="1:11" ht="15" customHeight="1">
+      <c r="A104" s="109">
+        <v>6</v>
+      </c>
+      <c r="B104" s="109" t="s">
+        <v>154</v>
+      </c>
+      <c r="C104" s="109"/>
+      <c r="D104" s="105"/>
+      <c r="E104" s="99"/>
+      <c r="F104" s="81"/>
+      <c r="G104" s="108"/>
+      <c r="I104" s="90"/>
+      <c r="J104" s="90"/>
+      <c r="K104" s="90"/>
+    </row>
+    <row r="105" spans="1:11" ht="68" customHeight="1">
+      <c r="A105" s="109">
+        <v>6.1</v>
+      </c>
+      <c r="B105" s="109"/>
+      <c r="C105" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="D105" s="105"/>
+      <c r="E105" s="99"/>
+      <c r="F105" s="81"/>
+      <c r="G105" s="108"/>
+      <c r="I105" s="90"/>
+      <c r="J105" s="90"/>
+      <c r="K105" s="90"/>
+    </row>
+    <row r="106" spans="1:11" ht="15" customHeight="1">
+      <c r="A106" s="109" t="s">
+        <v>24</v>
+      </c>
+      <c r="B106" s="109"/>
+      <c r="C106" s="79"/>
+      <c r="D106" s="105" t="s">
+        <v>29</v>
+      </c>
+      <c r="E106" s="99"/>
+      <c r="F106" s="81"/>
+      <c r="G106" s="108"/>
+      <c r="I106" s="90"/>
+      <c r="J106" s="90"/>
+      <c r="K106" s="90"/>
+    </row>
+    <row r="107" spans="1:11" ht="15" customHeight="1">
+      <c r="A107" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="B107" s="109"/>
+      <c r="C107" s="109"/>
+      <c r="D107" s="105" t="s">
+        <v>30</v>
+      </c>
+      <c r="E107" s="99"/>
+      <c r="F107" s="81"/>
+      <c r="G107" s="108"/>
+      <c r="I107" s="90"/>
+      <c r="J107" s="90"/>
+      <c r="K107" s="90"/>
+    </row>
+    <row r="108" spans="1:11" ht="15" customHeight="1">
+      <c r="A108" s="109" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="109"/>
+      <c r="C108" s="109"/>
+      <c r="D108" s="105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E108" s="99"/>
+      <c r="F108" s="81"/>
+      <c r="G108" s="108"/>
+      <c r="I108" s="90"/>
+      <c r="J108" s="90"/>
+      <c r="K108" s="90"/>
+    </row>
+    <row r="109" spans="1:11" ht="15" customHeight="1">
+      <c r="A109" s="109" t="s">
+        <v>27</v>
+      </c>
+      <c r="B109" s="109"/>
+      <c r="C109" s="109"/>
+      <c r="D109" s="105" t="s">
+        <v>32</v>
+      </c>
+      <c r="E109" s="99"/>
+      <c r="F109" s="81"/>
+      <c r="G109" s="108"/>
+      <c r="I109" s="90"/>
+      <c r="J109" s="90"/>
+      <c r="K109" s="90"/>
+    </row>
+    <row r="110" spans="1:11" ht="15" customHeight="1">
+      <c r="A110" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B110" s="29"/>
+      <c r="C110" s="29"/>
+      <c r="D110" s="105" t="s">
+        <v>34</v>
+      </c>
+      <c r="E110" s="99"/>
+      <c r="F110" s="81"/>
+      <c r="G110" s="108"/>
+      <c r="H110" s="92"/>
+      <c r="I110" s="90"/>
+      <c r="J110" s="90"/>
+      <c r="K110" s="90"/>
+    </row>
+    <row r="111" spans="1:11" ht="15" customHeight="1">
+      <c r="A111" s="95"/>
+      <c r="B111" s="95"/>
+      <c r="C111" s="95"/>
+      <c r="D111" s="105"/>
+      <c r="E111" s="99"/>
+      <c r="F111" s="81"/>
+      <c r="G111" s="108"/>
+      <c r="H111" s="92"/>
+      <c r="I111" s="90"/>
+      <c r="J111" s="90"/>
+      <c r="K111" s="90"/>
+    </row>
+    <row r="112" spans="1:11" ht="15" customHeight="1">
+      <c r="A112" s="95"/>
+      <c r="B112" s="95"/>
+      <c r="C112" s="95"/>
+      <c r="D112" s="105"/>
+      <c r="E112" s="99"/>
+      <c r="F112" s="81"/>
+      <c r="G112" s="108"/>
+      <c r="H112" s="92"/>
+      <c r="I112" s="90"/>
+      <c r="J112" s="90"/>
+      <c r="K112" s="90"/>
+    </row>
+    <row r="113" spans="1:11" ht="15" customHeight="1">
+      <c r="A113" s="95"/>
+      <c r="B113" s="95"/>
+      <c r="C113" s="95"/>
+      <c r="D113" s="105"/>
+      <c r="E113" s="99"/>
+      <c r="F113" s="81"/>
+      <c r="G113" s="108"/>
+      <c r="H113" s="92"/>
+      <c r="I113" s="90"/>
+      <c r="J113" s="90"/>
+      <c r="K113" s="90"/>
+    </row>
+    <row r="114" spans="1:11" ht="15" customHeight="1">
+      <c r="A114" s="95"/>
+      <c r="B114" s="95"/>
+      <c r="C114" s="95"/>
+      <c r="D114" s="105"/>
+      <c r="E114" s="99"/>
+      <c r="F114" s="81"/>
+      <c r="G114" s="108"/>
+      <c r="H114" s="92"/>
+      <c r="I114" s="90"/>
+      <c r="J114" s="90"/>
+      <c r="K114" s="90"/>
+    </row>
+    <row r="115" spans="1:11" ht="15" customHeight="1">
+      <c r="A115" s="95"/>
+      <c r="B115" s="95"/>
+      <c r="C115" s="95"/>
+      <c r="D115" s="105"/>
+      <c r="E115" s="99"/>
+      <c r="F115" s="81"/>
+      <c r="G115" s="108"/>
+      <c r="H115" s="92"/>
+      <c r="I115" s="90"/>
+      <c r="J115" s="90"/>
+      <c r="K115" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>